<commit_message>
Finished revising all suggestions and comments.
</commit_message>
<xml_diff>
--- a/Issues.xlsx
+++ b/Issues.xlsx
@@ -7,17 +7,17 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Status" sheetId="3" r:id="rId1"/>
+    <sheet name="2nd iteration" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Status!$B$2:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2nd iteration'!$B$2:$F$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="185">
   <si>
     <t>“Automation and Techniques” needs more explanation. Having read the whole document now I wonder if you mean “Automation and Development Techniques” or maybe “Automation and Technology”??</t>
   </si>
@@ -728,6 +728,22 @@
   </si>
   <si>
     <t>Deleted.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deleted.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I’d like to say it again here. This was the big experience for me.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deleted.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Added them on Introduction.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -767,18 +783,12 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -799,40 +809,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="56" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="56" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="56" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="56" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1138,9 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1175,59 +1171,59 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -1235,824 +1231,840 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.15">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="D18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.15">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="8" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.15">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="8" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="D24" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="4" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="4" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="4" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="D29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="4" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" x14ac:dyDescent="0.15">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="11" t="s">
+      <c r="D30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="D31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" s="8" t="s">
+      <c r="D32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="4" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E33" s="8" t="s">
+      <c r="D33" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="8" t="s">
+      <c r="D34" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="4" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="8" t="s">
+      <c r="D35" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="4" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E36" s="8" t="s">
+      <c r="D36" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="4" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E38" s="8" t="s">
+      <c r="D38" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="4" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="D39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E40" s="8" t="s">
+      <c r="D40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G40" s="4" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="D41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="9" t="s">
+      <c r="D42" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G42" s="7"/>
+      <c r="G42" s="4" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="43" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E43" s="8" t="s">
+      <c r="D43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="4" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9" t="s">
+      <c r="D44" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="3"/>
+      <c r="G44" s="4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="45" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9" t="s">
+      <c r="D45" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G45" s="3"/>
+      <c r="G45" s="4" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="46" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9" t="s">
+      <c r="D46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G46" s="3"/>
+      <c r="G46" s="4" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="47" spans="2:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="4" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>